<commit_message>
the new form is kinda working already
</commit_message>
<xml_diff>
--- a/fields.xlsx
+++ b/fields.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\bfpspc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070B7E5F-94C6-4174-BC79-0658103675AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966CFF42-9147-4F2B-82CC-28070F322DC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8310" yWindow="1095" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{F0EC362D-E276-4730-9B89-0A610901DD1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F0EC362D-E276-4730-9B89-0A610901DD1F}"/>
   </bookViews>
   <sheets>
     <sheet name="AFOR" sheetId="1" r:id="rId1"/>
     <sheet name="SPOT" sheetId="2" r:id="rId2"/>
+    <sheet name="New Incident" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -864,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB351E91-5E52-4AF8-BF63-56192AD785BC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -872,4 +873,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3248CA-515E-4A15-8D13-30CA4B5ABB84}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>